<commit_message>
[CODE] add temp CardStatistics
</commit_message>
<xml_diff>
--- a/depot/Log.xlsx
+++ b/depot/Log.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6">
   <si>
     <t>SA</t>
   </si>
@@ -29,18 +29,24 @@
   <si>
     <t>DA</t>
   </si>
+  <si>
+    <t>内裤</t>
+  </si>
+  <si>
+    <t>毛孔张开</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,6 +56,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -59,6 +72,59 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -73,35 +139,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -133,14 +170,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,24 +184,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -180,21 +194,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,187 +208,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,6 +426,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -442,17 +456,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -491,162 +499,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1002,15 +1001,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1022,6 +1021,62 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+      <c r="K1">
+        <v>52</v>
+      </c>
+      <c r="L1">
+        <v>2</v>
+      </c>
+      <c r="M1">
+        <f>COMBIN(K1,L1)</f>
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="2" spans="11:13">
+      <c r="K2">
+        <v>52</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <f>COMBIN(K2,L2)</f>
+        <v>270725</v>
+      </c>
+    </row>
+    <row r="4" spans="11:13">
+      <c r="K4">
+        <v>50</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <f>COMBIN(K4,L4)</f>
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="5" spans="11:13">
+      <c r="K5">
+        <v>48</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <f>COMBIN(K5,L5)</f>
+        <v>1712304</v>
+      </c>
+    </row>
+    <row r="8" spans="12:12">
+      <c r="L8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="12:12">
+      <c r="L9" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[CODE] optimize combination algorithm by pruning
</commit_message>
<xml_diff>
--- a/depot/Log.xlsx
+++ b/depot/Log.xlsx
@@ -30,7 +30,7 @@
     <t>DA</t>
   </si>
   <si>
-    <t>内裤</t>
+    <t>袜子</t>
   </si>
   <si>
     <t>毛孔张开</t>
@@ -41,9 +41,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -69,7 +69,74 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -92,15 +159,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -114,84 +175,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -208,19 +208,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -232,13 +310,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,13 +328,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,19 +346,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,103 +382,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,6 +399,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -413,6 +422,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -441,41 +465,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -491,11 +485,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,10 +507,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -519,133 +519,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1004,12 +1004,12 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1022,60 +1022,67 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="K1">
+    </row>
+    <row r="4" spans="9:13">
+      <c r="I4">
         <v>52</v>
       </c>
-      <c r="L1">
+      <c r="J4">
         <v>2</v>
       </c>
-      <c r="M1">
-        <f>COMBIN(K1,L1)</f>
+      <c r="K4">
+        <f>COMBIN(I4,J4)</f>
         <v>1326</v>
       </c>
+      <c r="M4">
+        <v>247</v>
+      </c>
     </row>
-    <row r="2" spans="11:13">
-      <c r="K2">
+    <row r="5" spans="9:13">
+      <c r="I5">
         <v>52</v>
       </c>
-      <c r="L2">
+      <c r="J5">
         <v>4</v>
       </c>
-      <c r="M2">
-        <f>COMBIN(K2,L2)</f>
+      <c r="K5">
+        <f>COMBIN(I5,J5)</f>
         <v>270725</v>
       </c>
+      <c r="M5">
+        <f>M4*K7</f>
+        <v>302575</v>
+      </c>
     </row>
-    <row r="4" spans="11:13">
-      <c r="K4">
+    <row r="7" spans="9:11">
+      <c r="I7">
         <v>50</v>
       </c>
-      <c r="L4">
+      <c r="J7">
         <v>2</v>
       </c>
-      <c r="M4">
-        <f>COMBIN(K4,L4)</f>
+      <c r="K7">
+        <f>COMBIN(I7,J7)</f>
         <v>1225</v>
       </c>
     </row>
-    <row r="5" spans="11:13">
-      <c r="K5">
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8">
         <v>48</v>
       </c>
-      <c r="L5">
+      <c r="J8">
         <v>5</v>
       </c>
-      <c r="M5">
-        <f>COMBIN(K5,L5)</f>
+      <c r="K8">
+        <f>COMBIN(I8,J8)</f>
         <v>1712304</v>
       </c>
     </row>
-    <row r="8" spans="12:12">
-      <c r="L8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="12:12">
-      <c r="L9" t="s">
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1092,7 +1099,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
[CODE] code nothing, go for switch!
</commit_message>
<xml_diff>
--- a/depot/Log.xlsx
+++ b/depot/Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="28695" windowHeight="12630"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25">
   <si>
     <t>handcard</t>
   </si>
@@ -39,7 +39,13 @@
     <t>SpadeSpade_VS_HeartHeart</t>
   </si>
   <si>
+    <t>SpadeHeart_VS_SpadeHeart</t>
+  </si>
+  <si>
     <t>SpadeSpade_VS_HeartClub</t>
+  </si>
+  <si>
+    <t>SpadeHeart_VS_SpadeClub</t>
   </si>
   <si>
     <t>SpadeHeart_VS_ClubDiamond</t>
@@ -93,9 +99,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -106,9 +112,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -123,45 +151,69 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -175,69 +227,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,25 +265,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,157 +403,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,6 +456,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -463,48 +493,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -525,17 +513,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -550,6 +547,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -558,10 +564,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -570,133 +576,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1059,7 +1065,7 @@
   <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1188,11 +1194,11 @@
         <v>55</v>
       </c>
       <c r="J7">
-        <f>COMBIN(H7,I7)</f>
+        <f t="shared" ref="J7:J11" si="1">COMBIN(H7,I7)</f>
         <v>1</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L7:L11" si="1">F7*J7</f>
+        <f t="shared" ref="L7:L11" si="2">F7*J7</f>
         <v>55</v>
       </c>
       <c r="N7">
@@ -1200,75 +1206,51 @@
         <v>4290</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>78</v>
-      </c>
-      <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="H8">
-        <v>13</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <f t="shared" ref="J8:J11" si="2">COMBIN(H8,I8)</f>
-        <v>13</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="1"/>
-        <v>130</v>
-      </c>
+    <row r="8" spans="14:14">
       <c r="N8">
-        <f>B8*L8</f>
-        <v>10140</v>
+        <f>B9*L9</f>
+        <v>11154</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>78</v>
       </c>
       <c r="D9">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>78</v>
+        <v>11</v>
+      </c>
+      <c r="H9">
+        <v>13</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
       </c>
       <c r="J9">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="L9">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="1"/>
-        <v>78</v>
+        <v>143</v>
       </c>
       <c r="N9">
-        <f>B9*L9</f>
+        <f>B10*L10</f>
         <v>6084</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>78</v>
@@ -1277,47 +1259,41 @@
         <v>13</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="H10">
-        <v>13</v>
-      </c>
-      <c r="I10">
+        <v>78</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="1"/>
-        <v>169</v>
+        <v>78</v>
       </c>
       <c r="N10">
-        <f>B10*L10</f>
+        <f>B14*L14</f>
         <v>13182</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>91</v>
       </c>
       <c r="D11">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H11">
         <v>13</v>
@@ -1326,91 +1302,189 @@
         <v>1</v>
       </c>
       <c r="J11">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="L11">
         <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="1"/>
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="N11">
-        <f>B11*L11</f>
+        <f>B17*L17</f>
         <v>15379</v>
       </c>
     </row>
-    <row r="12" spans="12:14">
-      <c r="L12">
-        <f>SUM(L7:L11)</f>
-        <v>601</v>
-      </c>
+    <row r="12" spans="14:14">
       <c r="N12">
         <f>SUM(N7:N11)</f>
-        <v>49075</v>
-      </c>
-    </row>
-    <row r="14" spans="4:5">
-      <c r="D14" t="s">
+        <v>50089</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>78</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f>COMBIN(D14,E14)</f>
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>13</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <f>COMBIN(H14,I14)</f>
+        <v>13</v>
+      </c>
+      <c r="L14">
+        <f>F14*J14</f>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="E14" t="s">
+      <c r="B15">
+        <v>91</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f>COMBIN(D15,E15)</f>
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <f>COMBIN(H15,I15)</f>
+        <v>13</v>
+      </c>
+      <c r="L15">
+        <f>F15*J15</f>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="4:6">
-      <c r="D15">
+      <c r="B17">
+        <v>91</v>
+      </c>
+      <c r="D17">
+        <v>13</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f>COMBIN(D17,E17)</f>
+        <v>13</v>
+      </c>
+      <c r="H17">
+        <v>13</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <f>COMBIN(H17,I17)</f>
+        <v>13</v>
+      </c>
+      <c r="L17">
+        <f>F17*J17</f>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="12:12">
+      <c r="L18">
+        <f>SUM(L7:L17)</f>
+        <v>926</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5">
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6">
+      <c r="D21">
         <v>16</v>
       </c>
-      <c r="E15">
+      <c r="E21">
         <v>16</v>
       </c>
-      <c r="F15">
-        <f>D15*E15</f>
+      <c r="F21">
+        <f>D21*E21</f>
         <v>256</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1493,17 +1567,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[CODE] start change a new way to CalcAllHandCardAgainstResult
</commit_message>
<xml_diff>
--- a/depot/Log.xlsx
+++ b/depot/Log.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="12630"/>
+    <workbookView windowWidth="19095" windowHeight="7830" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="handcard" sheetId="2" r:id="rId2"/>
-    <sheet name="game" sheetId="3" r:id="rId3"/>
+    <sheet name="Plan" sheetId="4" r:id="rId1"/>
+    <sheet name="design" sheetId="1" r:id="rId2"/>
+    <sheet name="handcard" sheetId="2" r:id="rId3"/>
+    <sheet name="game" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26">
   <si>
     <t>handcard</t>
   </si>
@@ -55,6 +56,9 @@
   </si>
   <si>
     <t>playerB</t>
+  </si>
+  <si>
+    <t>统计各种起手牌胜率</t>
   </si>
   <si>
     <t>毛孔张开</t>
@@ -98,15 +102,121 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -121,22 +231,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -150,93 +246,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,13 +259,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -265,187 +269,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,6 +460,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -474,11 +498,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -512,50 +560,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -564,10 +568,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -576,133 +580,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1062,10 +1066,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1442,49 +1462,62 @@
         <v>256</v>
       </c>
     </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24">
+        <v>1920</v>
+      </c>
+      <c r="C24">
+        <v>1080</v>
+      </c>
+    </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1494,7 +1527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:D4"/>
@@ -1554,7 +1587,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A2:A4"/>
@@ -1567,17 +1600,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>